<commit_message>
basic encoding kinda done
</commit_message>
<xml_diff>
--- a/truth_table.xlsx
+++ b/truth_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IITR Course Material\SEM 3\CSN-221 - Comp. Arch &amp; MP\Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489030AB-A995-4F7E-BCC6-CBA2C2247343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B7A46B-C9F9-4207-B2C7-F9DD8195E6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
   </bookViews>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9975F93C-2E30-4649-9A30-4C2FEF1CAB75}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1916,7 +1916,7 @@
         <v>57</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
simulator begins ig :)
</commit_message>
<xml_diff>
--- a/truth_table.xlsx
+++ b/truth_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IITR Course Material\SEM 3\CSN-221 - Comp. Arch &amp; MP\Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B7A46B-C9F9-4207-B2C7-F9DD8195E6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC26CE7F-2AE5-4A2D-BB60-B93BB69A3E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="92">
   <si>
     <t>Operation</t>
   </si>
   <si>
     <t>ALU Action</t>
-  </si>
-  <si>
-    <t>Opcode</t>
   </si>
   <si>
     <t>func3</t>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <t>0110011</t>
   </si>
   <si>
     <t>000</t>
@@ -195,16 +189,10 @@
     <t>I</t>
   </si>
   <si>
-    <t>0010011</t>
-  </si>
-  <si>
     <t>NIL</t>
   </si>
   <si>
     <t>lw</t>
-  </si>
-  <si>
-    <t>0000011</t>
   </si>
   <si>
     <t>010</t>
@@ -214,9 +202,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>0100011</t>
   </si>
   <si>
     <t>x</t>
@@ -249,25 +234,13 @@
     <t>J</t>
   </si>
   <si>
-    <t>1100011</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
     <t>I (spl)</t>
   </si>
   <si>
-    <t>1110011</t>
-  </si>
-  <si>
     <t>no encoding</t>
-  </si>
-  <si>
-    <t>0110111</t>
-  </si>
-  <si>
-    <t>0010111</t>
   </si>
   <si>
     <t>00</t>
@@ -295,6 +268,39 @@
   </si>
   <si>
     <t>ALUSel</t>
+  </si>
+  <si>
+    <t>Op5</t>
+  </si>
+  <si>
+    <t>01100</t>
+  </si>
+  <si>
+    <t>00100</t>
+  </si>
+  <si>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>01000</t>
+  </si>
+  <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>11011</t>
+  </si>
+  <si>
+    <t>11001</t>
+  </si>
+  <si>
+    <t>01101</t>
+  </si>
+  <si>
+    <t>00101</t>
+  </si>
+  <si>
+    <t>11100</t>
   </si>
 </sst>
 </file>
@@ -716,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9975F93C-2E30-4649-9A30-4C2FEF1CAB75}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,55 +754,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -813,58 +819,58 @@
     <row r="2" spans="1:30" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="L3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -881,58 +887,58 @@
     </row>
     <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -949,58 +955,58 @@
     </row>
     <row r="5" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -1017,58 +1023,58 @@
     </row>
     <row r="6" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1085,58 +1091,58 @@
     </row>
     <row r="7" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="J7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1153,58 +1159,58 @@
     </row>
     <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -1221,58 +1227,58 @@
     </row>
     <row r="9" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="J9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -1289,58 +1295,58 @@
     </row>
     <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -1357,58 +1363,58 @@
     </row>
     <row r="11" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1425,58 +1431,58 @@
     </row>
     <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="J12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O12" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1493,58 +1499,58 @@
     </row>
     <row r="13" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J13" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1561,58 +1567,58 @@
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -1629,58 +1635,58 @@
     </row>
     <row r="15" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1697,58 +1703,58 @@
     </row>
     <row r="16" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J16" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -1765,58 +1771,58 @@
     </row>
     <row r="17" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J17" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -1833,58 +1839,58 @@
     </row>
     <row r="18" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J18" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -1901,58 +1907,58 @@
     </row>
     <row r="19" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J19" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P19" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="Q19" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -1969,58 +1975,58 @@
     </row>
     <row r="20" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="P20" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -2037,58 +2043,58 @@
     </row>
     <row r="21" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R21" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2105,58 +2111,58 @@
     </row>
     <row r="22" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R22" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -2173,58 +2179,58 @@
     </row>
     <row r="23" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R23" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1101111</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -2241,58 +2247,58 @@
     </row>
     <row r="24" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1100111</v>
+        <v>54</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O24" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -2309,58 +2315,58 @@
     </row>
     <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="I25" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="N25" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -2377,58 +2383,58 @@
     </row>
     <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="N26" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -2445,22 +2451,22 @@
     </row>
     <row r="27" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="F27" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2468,25 +2474,25 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -33640,5 +33646,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
squashed killer bugs, single cycle cpu almost done, last commit before mte ig
</commit_message>
<xml_diff>
--- a/truth_table.xlsx
+++ b/truth_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IITR Course Material\SEM 3\CSN-221 - Comp. Arch &amp; MP\Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E6AA0F-9B39-47BE-AE5A-8A9B67952DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC2CFF1-35A0-4321-BA29-882ADB9E6AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9975F93C-2E30-4649-9A30-4C2FEF1CAB75}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2064,7 +2064,7 @@
         <v>17</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>78</v>
@@ -2132,7 +2132,7 @@
         <v>17</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
mte gone commits on
</commit_message>
<xml_diff>
--- a/truth_table.xlsx
+++ b/truth_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IITR Course Material\SEM 3\CSN-221 - Comp. Arch &amp; MP\Course-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC2CFF1-35A0-4321-BA29-882ADB9E6AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A59618-950B-454A-8EC8-9C30802C7EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{281143D4-4513-412F-83E3-71F070666CB2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="89">
   <si>
     <t>Operation</t>
   </si>
@@ -204,9 +204,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>beq</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>auipc</t>
   </si>
   <si>
-    <t>ecall</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -235,12 +229,6 @@
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>I (spl)</t>
-  </si>
-  <si>
-    <t>no encoding</t>
   </si>
   <si>
     <t>00</t>
@@ -297,10 +285,13 @@
     <t>00101</t>
   </si>
   <si>
-    <t>11100</t>
+    <t>ImmSel</t>
   </si>
   <si>
-    <t>ImmSel</t>
+    <t>li</t>
+  </si>
+  <si>
+    <t>pseudo</t>
   </si>
 </sst>
 </file>
@@ -722,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9975F93C-2E30-4649-9A30-4C2FEF1CAB75}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -769,19 +760,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -828,7 +819,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -846,7 +837,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>18</v>
@@ -867,10 +858,10 @@
         <v>17</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -896,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -914,7 +905,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>22</v>
@@ -935,10 +926,10 @@
         <v>17</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -964,7 +955,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
@@ -982,7 +973,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>25</v>
@@ -1003,10 +994,10 @@
         <v>17</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -1032,7 +1023,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
@@ -1050,7 +1041,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>28</v>
@@ -1071,10 +1062,10 @@
         <v>17</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1100,7 +1091,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -1118,7 +1109,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>36</v>
@@ -1139,10 +1130,10 @@
         <v>17</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1168,7 +1159,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
@@ -1186,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>38</v>
@@ -1207,10 +1198,10 @@
         <v>17</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -1236,7 +1227,7 @@
         <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>16</v>
@@ -1254,7 +1245,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>43</v>
@@ -1275,10 +1266,10 @@
         <v>17</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -1304,7 +1295,7 @@
         <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>42</v>
@@ -1322,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>44</v>
@@ -1343,10 +1334,10 @@
         <v>17</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -1372,7 +1363,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>42</v>
@@ -1390,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>45</v>
@@ -1411,10 +1402,10 @@
         <v>17</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1440,7 +1431,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>42</v>
@@ -1458,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>46</v>
@@ -1479,10 +1470,10 @@
         <v>17</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1508,7 +1499,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>54</v>
@@ -1526,7 +1517,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>18</v>
@@ -1547,10 +1538,10 @@
         <v>17</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1576,7 +1567,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>54</v>
@@ -1594,7 +1585,7 @@
         <v>21</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>25</v>
@@ -1615,10 +1606,10 @@
         <v>17</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -1644,7 +1635,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>54</v>
@@ -1662,7 +1653,7 @@
         <v>21</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>28</v>
@@ -1683,10 +1674,10 @@
         <v>17</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1712,7 +1703,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>54</v>
@@ -1730,7 +1721,7 @@
         <v>21</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>36</v>
@@ -1751,10 +1742,10 @@
         <v>17</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -1780,7 +1771,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>54</v>
@@ -1798,7 +1789,7 @@
         <v>21</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>38</v>
@@ -1819,10 +1810,10 @@
         <v>17</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -1848,7 +1839,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>54</v>
@@ -1866,7 +1857,7 @@
         <v>21</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>43</v>
@@ -1887,10 +1878,10 @@
         <v>17</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -1916,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>54</v>
@@ -1934,7 +1925,7 @@
         <v>21</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>18</v>
@@ -1955,10 +1946,10 @@
         <v>19</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -1984,7 +1975,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>54</v>
@@ -2002,7 +1993,7 @@
         <v>56</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>18</v>
@@ -2023,10 +2014,10 @@
         <v>17</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -2043,16 +2034,16 @@
     </row>
     <row r="21" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>54</v>
@@ -2067,10 +2058,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>22</v>
@@ -2091,10 +2082,10 @@
         <v>17</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2111,16 +2102,16 @@
     </row>
     <row r="22" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>54</v>
@@ -2135,10 +2126,10 @@
         <v>17</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>22</v>
@@ -2159,10 +2150,10 @@
         <v>17</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -2179,16 +2170,16 @@
     </row>
     <row r="23" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>54</v>
@@ -2206,7 +2197,7 @@
         <v>24</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>18</v>
@@ -2227,10 +2218,10 @@
         <v>17</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -2247,7 +2238,7 @@
     </row>
     <row r="24" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>53</v>
@@ -2256,7 +2247,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>54</v>
@@ -2274,7 +2265,7 @@
         <v>21</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>18</v>
@@ -2295,10 +2286,10 @@
         <v>17</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -2315,16 +2306,16 @@
     </row>
     <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>54</v>
@@ -2342,7 +2333,7 @@
         <v>40</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>18</v>
@@ -2363,10 +2354,10 @@
         <v>17</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -2383,16 +2374,16 @@
     </row>
     <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>54</v>
@@ -2410,7 +2401,7 @@
         <v>40</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>18</v>
@@ -2431,10 +2422,10 @@
         <v>17</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -2451,49 +2442,27 @@
     </row>
     <row r="27" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
-      <c r="L27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="R27" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="4"/>

</xml_diff>